<commit_message>
Completed Composition Pathology Report for Diagnostic Report FHIR IG
GitHub Fixes #19
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/composition-pathreport-1.xlsx
+++ b/output/DiagnosticReport/composition-pathreport-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2669" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2668" uniqueCount="476">
   <si>
     <t>Path</t>
   </si>
@@ -165,7 +165,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-dh-cmp-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-cmp-02:The author shall at least have a reference or an identifier with at least a system and a value {author.reference.exists() or author.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-cmp-03:The custodian shall at least have a reference or an identifier with at least a system and a value {custodian.reference.exists() or custodian.identifier.where(system.count() + value.count() &gt; 1).exists()}</t>
   </si>
   <si>
     <t>Event</t>
@@ -221,81 +221,85 @@
     <t>Resource.meta</t>
   </si>
   <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+inv-dh-cmp-04:One profile shall be 'http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/composition-pathreport-1' {profile.where($this='http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/composition-pathreport-1').exists()}</t>
+  </si>
+  <si>
+    <t>Composition.meta.id</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Composition.meta.extension</t>
+  </si>
+  <si>
+    <t>extensions
+user content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>Composition.meta.versionId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id
+</t>
+  </si>
+  <si>
+    <t>Version specific identifier</t>
+  </si>
+  <si>
+    <t>The version specific identifier, as it appears in the version portion of the URL. This value changes when the resource is created, updated, or deleted.</t>
+  </si>
+  <si>
+    <t>The server assigns this value, and ignores what the client specifies, except in the case that the server is imposing version integrity on updates/deletes.</t>
+  </si>
+  <si>
+    <t>Meta.versionId</t>
+  </si>
+  <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
   </si>
   <si>
-    <t>Composition.meta.id</t>
-  </si>
-  <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>Composition.meta.extension</t>
-  </si>
-  <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension
-</t>
-  </si>
-  <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>Composition.meta.versionId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id
-</t>
-  </si>
-  <si>
-    <t>Version specific identifier</t>
-  </si>
-  <si>
-    <t>The version specific identifier, as it appears in the version portion of the URL. This value changes when the resource is created, updated, or deleted.</t>
-  </si>
-  <si>
-    <t>The server assigns this value, and ignores what the client specifies, except in the case that the server is imposing version integrity on updates/deletes.</t>
-  </si>
-  <si>
-    <t>Meta.versionId</t>
-  </si>
-  <si>
     <t>Composition.meta.lastUpdated</t>
   </si>
   <si>
@@ -583,7 +587,7 @@
     <t>Composition.status</t>
   </si>
   <si>
-    <t>preliminary | final | amended | entered-in-error</t>
+    <t>preliminary | final | amended</t>
   </si>
   <si>
     <t>The workflow/clinical status of this composition. The status is a marker for the clinical standing of the document.</t>
@@ -599,10 +603,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>The workflow/clinical status of the composition.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/composition-status|4.0.1</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/compositionstatus-document-available-1</t>
   </si>
   <si>
     <t>Event.status</t>
@@ -698,7 +699,7 @@
     <t>Composition.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/patient-mhr-1|http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/patient-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-mhr-1|http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-ident-1)
 </t>
   </si>
   <si>
@@ -794,7 +795,7 @@
     <t>Composition.author</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/practitionerrole-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/practitionerrole-ident-1)
 </t>
   </si>
   <si>
@@ -886,6 +887,10 @@
     <t>Identifies responsibility for the accuracy of the composition content.</t>
   </si>
   <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+inv-dh-cmp-05:The party shall at least have a reference or an identifier with at least a system and a value {party.reference.exists() or party.identifier.where(system.count() + value.count() &gt; 1).exists()}</t>
+  </si>
+  <si>
     <t>.participation[typeCode="AUTHEN"].role[classCode="ASSIGNED"]</t>
   </si>
   <si>
@@ -987,7 +992,7 @@
     <t>Composition.custodian</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/organization-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/organization-ident-1)
 </t>
   </si>
   <si>
@@ -1679,7 +1684,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.7734375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="73.27734375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="82.76171875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
@@ -2519,7 +2524,7 @@
         <v>43</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ7" t="s" s="2">
         <v>43</v>
@@ -2545,7 +2550,7 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
@@ -2568,16 +2573,16 @@
         <v>56</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -2627,7 +2632,7 @@
         <v>43</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>44</v>
@@ -2639,7 +2644,7 @@
         <v>43</v>
       </c>
       <c r="AI8" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ8" t="s" s="2">
         <v>43</v>
@@ -2665,7 +2670,7 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -2688,16 +2693,16 @@
         <v>56</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -2747,7 +2752,7 @@
         <v>43</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>44</v>
@@ -2759,7 +2764,7 @@
         <v>43</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ9" t="s" s="2">
         <v>43</v>
@@ -2785,7 +2790,7 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
@@ -2808,16 +2813,16 @@
         <v>56</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
@@ -2867,7 +2872,7 @@
         <v>43</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>44</v>
@@ -2879,7 +2884,7 @@
         <v>43</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>43</v>
@@ -2905,7 +2910,7 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -2928,16 +2933,16 @@
         <v>56</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
@@ -2963,13 +2968,13 @@
         <v>43</v>
       </c>
       <c r="W11" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Z11" t="s" s="2">
         <v>43</v>
@@ -2987,7 +2992,7 @@
         <v>43</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>44</v>
@@ -2999,7 +3004,7 @@
         <v>43</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ11" t="s" s="2">
         <v>43</v>
@@ -3025,7 +3030,7 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -3048,16 +3053,16 @@
         <v>56</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
@@ -3083,13 +3088,13 @@
         <v>43</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="Z12" t="s" s="2">
         <v>43</v>
@@ -3107,7 +3112,7 @@
         <v>43</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>44</v>
@@ -3119,7 +3124,7 @@
         <v>43</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ12" t="s" s="2">
         <v>43</v>
@@ -3145,7 +3150,7 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -3168,16 +3173,16 @@
         <v>56</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
@@ -3227,7 +3232,7 @@
         <v>43</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>44</v>
@@ -3239,7 +3244,7 @@
         <v>43</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ13" t="s" s="2">
         <v>43</v>
@@ -3265,7 +3270,7 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -3288,16 +3293,16 @@
         <v>43</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -3305,7 +3310,7 @@
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="R14" t="s" s="2">
         <v>43</v>
@@ -3323,13 +3328,13 @@
         <v>43</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>43</v>
@@ -3347,7 +3352,7 @@
         <v>43</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>44</v>
@@ -3359,7 +3364,7 @@
         <v>43</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ14" t="s" s="2">
         <v>43</v>
@@ -3385,11 +3390,11 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
@@ -3408,16 +3413,16 @@
         <v>43</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
@@ -3467,7 +3472,7 @@
         <v>43</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>44</v>
@@ -3479,7 +3484,7 @@
         <v>43</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ15" t="s" s="2">
         <v>43</v>
@@ -3488,7 +3493,7 @@
         <v>43</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AM15" t="s" s="2">
         <v>43</v>
@@ -3505,11 +3510,11 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -3528,16 +3533,16 @@
         <v>43</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -3587,7 +3592,7 @@
         <v>43</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>44</v>
@@ -3608,7 +3613,7 @@
         <v>43</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AM16" t="s" s="2">
         <v>43</v>
@@ -3625,7 +3630,7 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3651,10 +3656,10 @@
         <v>75</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -3703,7 +3708,7 @@
         <v>81</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>44</v>
@@ -3741,10 +3746,10 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s" s="2">
         <v>43</v>
@@ -3766,13 +3771,13 @@
         <v>43</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3823,7 +3828,7 @@
         <v>43</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>44</v>
@@ -3832,7 +3837,7 @@
         <v>45</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AI18" t="s" s="2">
         <v>83</v>
@@ -3861,7 +3866,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3887,16 +3892,16 @@
         <v>75</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="M19" t="s" s="2">
         <v>78</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>43</v>
@@ -3945,7 +3950,7 @@
         <v>43</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>44</v>
@@ -3966,7 +3971,7 @@
         <v>43</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AM19" t="s" s="2">
         <v>43</v>
@@ -3983,7 +3988,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -4006,16 +4011,16 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -4065,7 +4070,7 @@
         <v>43</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>44</v>
@@ -4077,33 +4082,33 @@
         <v>43</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AN20" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AO20" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="AP20" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -4126,19 +4131,19 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>43</v>
@@ -4163,11 +4168,9 @@
         <v>43</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="X21" t="s" s="2">
         <v>186</v>
       </c>
+      <c r="X21" s="2"/>
       <c r="Y21" t="s" s="2">
         <v>187</v>
       </c>
@@ -4187,7 +4190,7 @@
         <v>43</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>55</v>
@@ -4199,7 +4202,7 @@
         <v>43</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ21" t="s" s="2">
         <v>188</v>
@@ -4285,7 +4288,7 @@
         <v>43</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="X22" t="s" s="2">
         <v>199</v>
@@ -4321,7 +4324,7 @@
         <v>43</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ22" t="s" s="2">
         <v>201</v>
@@ -4407,7 +4410,7 @@
         <v>43</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="X23" t="s" s="2">
         <v>211</v>
@@ -4443,7 +4446,7 @@
         <v>43</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>213</v>
@@ -4565,7 +4568,7 @@
         <v>43</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>43</v>
@@ -4685,7 +4688,7 @@
         <v>43</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>231</v>
@@ -4807,7 +4810,7 @@
         <v>43</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ26" t="s" s="2">
         <v>242</v>
@@ -4927,7 +4930,7 @@
         <v>43</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ27" t="s" s="2">
         <v>252</v>
@@ -5047,7 +5050,7 @@
         <v>43</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ28" t="s" s="2">
         <v>43</v>
@@ -5096,7 +5099,7 @@
         <v>56</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K29" t="s" s="2">
         <v>265</v>
@@ -5131,7 +5134,7 @@
         <v>43</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="X29" t="s" s="2">
         <v>268</v>
@@ -5167,7 +5170,7 @@
         <v>43</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ29" t="s" s="2">
         <v>43</v>
@@ -5289,7 +5292,7 @@
         <v>43</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>67</v>
+        <v>278</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>43</v>
@@ -5298,7 +5301,7 @@
         <v>43</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>43</v>
@@ -5307,15 +5310,15 @@
         <v>43</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AP30" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5433,7 +5436,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5553,11 +5556,11 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
@@ -5579,16 +5582,16 @@
         <v>75</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>78</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>43</v>
@@ -5637,7 +5640,7 @@
         <v>43</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>44</v>
@@ -5658,7 +5661,7 @@
         <v>43</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>43</v>
@@ -5675,7 +5678,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5698,24 +5701,24 @@
         <v>43</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>43</v>
       </c>
       <c r="P34" s="2"/>
       <c r="Q34" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="R34" t="s" s="2">
         <v>43</v>
@@ -5733,13 +5736,13 @@
         <v>43</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>43</v>
@@ -5757,7 +5760,7 @@
         <v>43</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>55</v>
@@ -5769,7 +5772,7 @@
         <v>43</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ34" t="s" s="2">
         <v>43</v>
@@ -5778,7 +5781,7 @@
         <v>43</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>43</v>
@@ -5787,7 +5790,7 @@
         <v>43</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AP34" t="s" s="2">
         <v>43</v>
@@ -5795,7 +5798,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5821,14 +5824,14 @@
         <v>237</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>43</v>
@@ -5877,7 +5880,7 @@
         <v>43</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>44</v>
@@ -5889,7 +5892,7 @@
         <v>43</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>43</v>
@@ -5898,7 +5901,7 @@
         <v>43</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>43</v>
@@ -5907,7 +5910,7 @@
         <v>43</v>
       </c>
       <c r="AO35" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AP35" t="s" s="2">
         <v>43</v>
@@ -5915,7 +5918,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5941,14 +5944,14 @@
         <v>248</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>43</v>
@@ -5997,7 +6000,7 @@
         <v>43</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>44</v>
@@ -6009,7 +6012,7 @@
         <v>43</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>43</v>
@@ -6018,16 +6021,16 @@
         <v>43</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AO36" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AP36" t="s" s="2">
         <v>43</v>
@@ -6035,7 +6038,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -6058,19 +6061,19 @@
         <v>56</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>43</v>
@@ -6119,7 +6122,7 @@
         <v>43</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>44</v>
@@ -6131,7 +6134,7 @@
         <v>43</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>43</v>
@@ -6140,7 +6143,7 @@
         <v>43</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>43</v>
@@ -6149,15 +6152,15 @@
         <v>43</v>
       </c>
       <c r="AO37" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AP37" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -6183,13 +6186,13 @@
         <v>273</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
@@ -6239,7 +6242,7 @@
         <v>43</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>44</v>
@@ -6251,7 +6254,7 @@
         <v>43</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>43</v>
@@ -6260,7 +6263,7 @@
         <v>43</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>43</v>
@@ -6269,15 +6272,15 @@
         <v>43</v>
       </c>
       <c r="AO38" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AP38" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6395,7 +6398,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6515,11 +6518,11 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
@@ -6541,16 +6544,16 @@
         <v>75</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M41" t="s" s="2">
         <v>78</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>43</v>
@@ -6599,7 +6602,7 @@
         <v>43</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>44</v>
@@ -6620,7 +6623,7 @@
         <v>43</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>43</v>
@@ -6637,7 +6640,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6660,16 +6663,16 @@
         <v>43</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6695,13 +6698,13 @@
         <v>43</v>
       </c>
       <c r="W42" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>43</v>
@@ -6719,7 +6722,7 @@
         <v>43</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>55</v>
@@ -6731,7 +6734,7 @@
         <v>43</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>43</v>
@@ -6740,7 +6743,7 @@
         <v>43</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>43</v>
@@ -6749,15 +6752,15 @@
         <v>43</v>
       </c>
       <c r="AO42" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AP42" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6780,13 +6783,13 @@
         <v>43</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -6837,7 +6840,7 @@
         <v>43</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>55</v>
@@ -6849,7 +6852,7 @@
         <v>43</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>43</v>
@@ -6858,7 +6861,7 @@
         <v>43</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>43</v>
@@ -6867,15 +6870,15 @@
         <v>43</v>
       </c>
       <c r="AO43" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AP43" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6901,16 +6904,16 @@
         <v>273</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>43</v>
@@ -6959,7 +6962,7 @@
         <v>43</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>44</v>
@@ -6971,7 +6974,7 @@
         <v>43</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ44" t="s" s="2">
         <v>43</v>
@@ -6980,7 +6983,7 @@
         <v>43</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AM44" t="s" s="2">
         <v>43</v>
@@ -6989,15 +6992,15 @@
         <v>43</v>
       </c>
       <c r="AO44" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AP44" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -7115,7 +7118,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -7235,11 +7238,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -7261,16 +7264,16 @@
         <v>75</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M47" t="s" s="2">
         <v>78</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>43</v>
@@ -7319,7 +7322,7 @@
         <v>43</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>44</v>
@@ -7340,7 +7343,7 @@
         <v>43</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AM47" t="s" s="2">
         <v>43</v>
@@ -7357,7 +7360,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7383,13 +7386,13 @@
         <v>193</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -7415,13 +7418,13 @@
         <v>43</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>43</v>
@@ -7439,7 +7442,7 @@
         <v>43</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>44</v>
@@ -7451,7 +7454,7 @@
         <v>43</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>43</v>
@@ -7472,12 +7475,12 @@
         <v>204</v>
       </c>
       <c r="AP48" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7500,13 +7503,13 @@
         <v>56</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -7557,7 +7560,7 @@
         <v>43</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>44</v>
@@ -7569,7 +7572,7 @@
         <v>43</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>43</v>
@@ -7590,12 +7593,12 @@
         <v>245</v>
       </c>
       <c r="AP49" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7618,13 +7621,13 @@
         <v>56</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -7675,7 +7678,7 @@
         <v>43</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>44</v>
@@ -7687,7 +7690,7 @@
         <v>43</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>43</v>
@@ -7696,7 +7699,7 @@
         <v>43</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AM50" t="s" s="2">
         <v>43</v>
@@ -7713,7 +7716,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7739,10 +7742,10 @@
         <v>273</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -7793,7 +7796,7 @@
         <v>43</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>44</v>
@@ -7805,7 +7808,7 @@
         <v>43</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>43</v>
@@ -7814,7 +7817,7 @@
         <v>43</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>43</v>
@@ -7823,7 +7826,7 @@
         <v>43</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AP51" t="s" s="2">
         <v>43</v>
@@ -7831,7 +7834,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7949,7 +7952,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -8069,11 +8072,11 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
@@ -8095,16 +8098,16 @@
         <v>75</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M54" t="s" s="2">
         <v>78</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>43</v>
@@ -8153,7 +8156,7 @@
         <v>43</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>44</v>
@@ -8174,7 +8177,7 @@
         <v>43</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>43</v>
@@ -8191,11 +8194,11 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -8217,16 +8220,16 @@
         <v>57</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>43</v>
@@ -8275,7 +8278,7 @@
         <v>43</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>44</v>
@@ -8287,7 +8290,7 @@
         <v>43</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>43</v>
@@ -8313,7 +8316,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8339,16 +8342,16 @@
         <v>193</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>43</v>
@@ -8358,7 +8361,7 @@
         <v>43</v>
       </c>
       <c r="R56" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="S56" t="s" s="2">
         <v>43</v>
@@ -8373,13 +8376,13 @@
         <v>43</v>
       </c>
       <c r="W56" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="Z56" t="s" s="2">
         <v>43</v>
@@ -8397,7 +8400,7 @@
         <v>43</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>44</v>
@@ -8409,7 +8412,7 @@
         <v>43</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ56" t="s" s="2">
         <v>43</v>
@@ -8435,7 +8438,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8458,13 +8461,13 @@
         <v>43</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" t="s" s="2">
@@ -8517,7 +8520,7 @@
         <v>43</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>44</v>
@@ -8529,7 +8532,7 @@
         <v>43</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ57" t="s" s="2">
         <v>43</v>
@@ -8555,7 +8558,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8578,16 +8581,16 @@
         <v>43</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
@@ -8637,7 +8640,7 @@
         <v>43</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>44</v>
@@ -8649,7 +8652,7 @@
         <v>43</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ58" t="s" s="2">
         <v>43</v>
@@ -8667,7 +8670,7 @@
         <v>43</v>
       </c>
       <c r="AO58" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AP58" t="s" s="2">
         <v>43</v>
@@ -8675,7 +8678,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8698,16 +8701,16 @@
         <v>43</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
@@ -8757,7 +8760,7 @@
         <v>43</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>44</v>
@@ -8766,10 +8769,10 @@
         <v>55</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ59" t="s" s="2">
         <v>43</v>
@@ -8778,7 +8781,7 @@
         <v>43</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AM59" t="s" s="2">
         <v>43</v>
@@ -8787,7 +8790,7 @@
         <v>43</v>
       </c>
       <c r="AO59" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AP59" t="s" s="2">
         <v>43</v>
@@ -8795,7 +8798,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8818,26 +8821,26 @@
         <v>43</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>43</v>
       </c>
       <c r="P60" s="2"/>
       <c r="Q60" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="R60" t="s" s="2">
         <v>43</v>
@@ -8855,13 +8858,13 @@
         <v>43</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>43</v>
@@ -8879,7 +8882,7 @@
         <v>43</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>44</v>
@@ -8891,7 +8894,7 @@
         <v>43</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ60" t="s" s="2">
         <v>43</v>
@@ -8900,7 +8903,7 @@
         <v>43</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AM60" t="s" s="2">
         <v>203</v>
@@ -8917,7 +8920,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8943,16 +8946,16 @@
         <v>193</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>43</v>
@@ -8977,13 +8980,13 @@
         <v>43</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>43</v>
@@ -9001,7 +9004,7 @@
         <v>43</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>44</v>
@@ -9013,7 +9016,7 @@
         <v>43</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>43</v>
@@ -9022,7 +9025,7 @@
         <v>43</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>43</v>
@@ -9039,7 +9042,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -9062,16 +9065,16 @@
         <v>43</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -9121,7 +9124,7 @@
         <v>43</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>44</v>
@@ -9130,10 +9133,10 @@
         <v>45</v>
       </c>
       <c r="AH62" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ62" t="s" s="2">
         <v>43</v>
@@ -9142,7 +9145,7 @@
         <v>43</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>43</v>
@@ -9151,7 +9154,7 @@
         <v>43</v>
       </c>
       <c r="AO62" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AP62" t="s" s="2">
         <v>43</v>
@@ -9159,7 +9162,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -9277,7 +9280,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9397,7 +9400,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9423,13 +9426,13 @@
         <v>57</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
@@ -9479,7 +9482,7 @@
         <v>43</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>44</v>
@@ -9488,10 +9491,10 @@
         <v>55</v>
       </c>
       <c r="AH65" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="AI65" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ65" t="s" s="2">
         <v>43</v>
@@ -9500,7 +9503,7 @@
         <v>43</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AM65" t="s" s="2">
         <v>43</v>
@@ -9517,7 +9520,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9540,16 +9543,16 @@
         <v>56</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
@@ -9575,13 +9578,13 @@
         <v>43</v>
       </c>
       <c r="W66" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="Z66" t="s" s="2">
         <v>43</v>
@@ -9599,7 +9602,7 @@
         <v>43</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>44</v>
@@ -9611,7 +9614,7 @@
         <v>43</v>
       </c>
       <c r="AI66" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ66" t="s" s="2">
         <v>43</v>
@@ -9620,7 +9623,7 @@
         <v>43</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>43</v>
@@ -9637,7 +9640,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9660,16 +9663,16 @@
         <v>56</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
@@ -9719,7 +9722,7 @@
         <v>43</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>44</v>
@@ -9731,7 +9734,7 @@
         <v>43</v>
       </c>
       <c r="AI67" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ67" t="s" s="2">
         <v>43</v>
@@ -9740,7 +9743,7 @@
         <v>43</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>43</v>
@@ -9757,7 +9760,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9783,13 +9786,13 @@
         <v>57</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
@@ -9839,7 +9842,7 @@
         <v>43</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>44</v>
@@ -9851,7 +9854,7 @@
         <v>43</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ68" t="s" s="2">
         <v>43</v>
@@ -9860,7 +9863,7 @@
         <v>43</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AM68" t="s" s="2">
         <v>43</v>
@@ -9877,7 +9880,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9903,16 +9906,16 @@
         <v>193</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="N69" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>43</v>
@@ -9937,13 +9940,13 @@
         <v>43</v>
       </c>
       <c r="W69" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="X69" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="Y69" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="Z69" t="s" s="2">
         <v>43</v>
@@ -9961,7 +9964,7 @@
         <v>43</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>44</v>
@@ -9970,10 +9973,10 @@
         <v>55</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AI69" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ69" t="s" s="2">
         <v>43</v>
@@ -9982,7 +9985,7 @@
         <v>43</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="AM69" t="s" s="2">
         <v>43</v>
@@ -9999,7 +10002,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -10025,13 +10028,13 @@
         <v>43</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
@@ -10081,7 +10084,7 @@
         <v>43</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>44</v>
@@ -10090,10 +10093,10 @@
         <v>45</v>
       </c>
       <c r="AH70" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AI70" t="s" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="AJ70" t="s" s="2">
         <v>43</v>
@@ -10102,7 +10105,7 @@
         <v>43</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AM70" t="s" s="2">
         <v>43</v>
@@ -10111,7 +10114,7 @@
         <v>43</v>
       </c>
       <c r="AO70" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="AP70" t="s" s="2">
         <v>43</v>

</xml_diff>